<commit_message>
Fix schematic and update 3d models
</commit_message>
<xml_diff>
--- a/hopper-power-dist-bom.xlsx
+++ b/hopper-power-dist-bom.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\git_workspace\hopper-power-dist\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E513B9D7-FFB7-4170-BB7D-F8B168B5635D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36A44824-7B1B-4613-A5AD-288CB7B3B91E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="75">
   <si>
     <t>Component Count:</t>
   </si>
@@ -52,12 +52,6 @@
     <t>Polarized capacitor</t>
   </si>
   <si>
-    <t xml:space="preserve">C4, C5, C6, </t>
-  </si>
-  <si>
-    <t xml:space="preserve">C7, C8, C9, C10, </t>
-  </si>
-  <si>
     <t xml:space="preserve">D1, </t>
   </si>
   <si>
@@ -178,12 +172,6 @@
     <t>https://www.mouser.com/ProductDetail/NKK-Switches/G3T12AB?qs=KqcCwYXy5KFsWJ9JmItWQA%3D%3D</t>
   </si>
   <si>
-    <t>https://www.mouser.com/ProductDetail/Vishay-BC-Components/MAL214699904E3?qs=2cdrMlin3n2weZkz3wC%2FLw%3D%3D</t>
-  </si>
-  <si>
-    <t>https://www.mouser.com/ProductDetail/Nichicon/UUX2G010MNL1GS?qs=aoAypCcaRa%2FXm3BGeiMtMQ%3D%3D</t>
-  </si>
-  <si>
     <t>https://www.mouser.com/ProductDetail/Vishay-BC-Components/MAL214699903E3?qs=sGAEpiMZZMsh%252B1woXyUXjzDUHoE4k%252BEHRBzY3jTxpCc%3D</t>
   </si>
   <si>
@@ -233,6 +221,30 @@
   </si>
   <si>
     <t>(CONNECTS TO J8, NOT SHOWN ON SCHEMATIC/BOARD)</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Taiyo-Yuden/HMK316B7105KL8T?qs=hWgE7mdIu5QAYJ6vxKB7KA%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/TDK/CKG57KX7R1E476M335JJ?qs=%2FP2Ij7fVdhEqTsqETKQplg%3D%3D</t>
+  </si>
+  <si>
+    <t>Capacitor</t>
+  </si>
+  <si>
+    <t>Capacitor_SMD:C_2220_5650Metric</t>
+  </si>
+  <si>
+    <t>Capacitor_SMD:C_1206_3216Metric</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>C5, C6, C7, C8,</t>
   </si>
 </sst>
 </file>
@@ -1088,7 +1100,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1120,7 +1132,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>2</v>
@@ -1135,7 +1147,7 @@
         <v>5</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -1146,24 +1158,24 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>73</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>72</v>
       </c>
       <c r="E3" t="s">
-        <v>9</v>
+        <v>70</v>
       </c>
       <c r="F3" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>67</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -1178,285 +1190,285 @@
         <v>9</v>
       </c>
       <c r="F4" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>74</v>
       </c>
       <c r="B5">
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>73</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
+        <v>71</v>
       </c>
       <c r="E5" t="s">
-        <v>9</v>
+        <v>70</v>
       </c>
       <c r="F5" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>52</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F6" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B7">
         <v>3</v>
       </c>
       <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" t="s">
         <v>16</v>
       </c>
-      <c r="D7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" t="s">
-        <v>18</v>
-      </c>
       <c r="F7" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
       <c r="C8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" t="s">
         <v>20</v>
       </c>
-      <c r="D8" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" t="s">
-        <v>22</v>
-      </c>
       <c r="F8" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B9">
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F9" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B10">
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E10" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="F10" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B11">
         <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D11" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F11" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
       <c r="C12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" t="s">
         <v>33</v>
       </c>
-      <c r="D12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E12" t="s">
-        <v>35</v>
-      </c>
       <c r="F12" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B13">
         <v>3</v>
       </c>
       <c r="C13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13" t="s">
         <v>37</v>
       </c>
-      <c r="D13" t="s">
-        <v>38</v>
-      </c>
-      <c r="E13" t="s">
-        <v>39</v>
-      </c>
       <c r="F13" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
       <c r="C14" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" t="s">
         <v>37</v>
       </c>
-      <c r="D14" t="s">
-        <v>41</v>
-      </c>
-      <c r="E14" t="s">
-        <v>39</v>
-      </c>
       <c r="F14" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D15" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E15" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F15" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D16" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E16" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="F16" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E17" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F17" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1464,15 +1476,13 @@
     <hyperlink ref="G12" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="G14" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
     <hyperlink ref="G15" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="G3" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="G4" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="G5" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="G6" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="G8" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="G7" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="G13" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="G9" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="G17" r:id="rId12" xr:uid="{8C7EB9BF-0CBB-4B4A-AC2E-C0E44EE43721}"/>
+    <hyperlink ref="G4" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="G6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="G8" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="G7" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="G13" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="G9" r:id="rId9" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="G17" r:id="rId10" xr:uid="{8C7EB9BF-0CBB-4B4A-AC2E-C0E44EE43721}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Improved PCB design and completed DRC
</commit_message>
<xml_diff>
--- a/hopper-power-dist-bom.xlsx
+++ b/hopper-power-dist-bom.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\git_workspace\hopper-power-dist\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\git_workspace\hopper-power-dist\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36A44824-7B1B-4613-A5AD-288CB7B3B91E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="hopper-power-dist" sheetId="1" r:id="rId1"/>
@@ -250,7 +249,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1096,11 +1095,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1473,16 +1472,18 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G12" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="G14" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="G15" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="G4" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="G6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="G8" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="G7" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="G13" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="G9" r:id="rId9" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="G17" r:id="rId10" xr:uid="{8C7EB9BF-0CBB-4B4A-AC2E-C0E44EE43721}"/>
+    <hyperlink ref="G12" r:id="rId1"/>
+    <hyperlink ref="G14" r:id="rId2"/>
+    <hyperlink ref="G15" r:id="rId3"/>
+    <hyperlink ref="G4" r:id="rId4"/>
+    <hyperlink ref="G6" r:id="rId5"/>
+    <hyperlink ref="G8" r:id="rId6"/>
+    <hyperlink ref="G7" r:id="rId7"/>
+    <hyperlink ref="G13" r:id="rId8"/>
+    <hyperlink ref="G9" r:id="rId9"/>
+    <hyperlink ref="G17" r:id="rId10"/>
+    <hyperlink ref="G3" r:id="rId11"/>
+    <hyperlink ref="G5" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Replaced DC-DC Converter and working on capacitor selection
</commit_message>
<xml_diff>
--- a/hopper-power-dist-bom.xlsx
+++ b/hopper-power-dist-bom.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\git_workspace\hopper-power-dist\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63DF09C9-9543-4813-8533-ECB8F76A410E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4928F5E-D88D-478E-892F-7BC67C03DA30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -210,9 +210,6 @@
     <t xml:space="preserve">S1, </t>
   </si>
   <si>
-    <t>G3T12AB</t>
-  </si>
-  <si>
     <t>NKK Switches SPDT Toggle Switch, On-On, Surface Mount</t>
   </si>
   <si>
@@ -250,6 +247,9 @@
   </si>
   <si>
     <t>ULT-12_2.5-D48N-C</t>
+  </si>
+  <si>
+    <t>2MS6T1B3M2QES</t>
   </si>
 </sst>
 </file>
@@ -324,10 +324,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="2" applyFont="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Excel Built-in Check Cell" xfId="2" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
@@ -715,7 +716,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -968,10 +969,10 @@
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E12" t="s">
         <v>51</v>
@@ -980,7 +981,7 @@
         <v>12</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1037,53 +1038,53 @@
         <v>1</v>
       </c>
       <c r="C15" t="s">
+        <v>74</v>
+      </c>
+      <c r="D15" t="s">
+        <v>74</v>
+      </c>
+      <c r="E15" t="s">
         <v>61</v>
-      </c>
-      <c r="D15" t="s">
-        <v>61</v>
-      </c>
-      <c r="E15" t="s">
-        <v>62</v>
       </c>
       <c r="F15" t="s">
         <v>12</v>
       </c>
-      <c r="G15" s="2" t="s">
-        <v>63</v>
+      <c r="G15" s="3" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
       <c r="C16" t="s">
+        <v>64</v>
+      </c>
+      <c r="D16" t="s">
         <v>65</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>66</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>67</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" s="2" t="s">
         <v>68</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="17" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F17" t="s">
         <v>45</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1098,6 +1099,7 @@
     <hyperlink ref="G13" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
     <hyperlink ref="G14" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
     <hyperlink ref="G17" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="G15" r:id="rId11" xr:uid="{EFA46D19-77E3-4293-BE84-A789C163AE0C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>